<commit_message>
Fix incorrect column header
</commit_message>
<xml_diff>
--- a/data/defaultInputValues.xlsx
+++ b/data/defaultInputValues.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">stochastic</t>
   </si>
   <si>
-    <t xml:space="preserve">vitalStatistics</t>
+    <t xml:space="preserve">vitalDynamics</t>
   </si>
   <si>
     <t xml:space="preserve">massAction</t>
@@ -311,7 +311,7 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,7 +380,7 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -484,7 +484,7 @@
         <v>0.00178</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>2.73</v>
+        <v>0.00273</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>

</xml_diff>